<commit_message>
updated locators in sample excel file
</commit_message>
<xml_diff>
--- a/CoreInteractions_Specs.xlsx
+++ b/CoreInteractions_Specs.xlsx
@@ -123,9 +123,6 @@
     <t>tooltip of selected bubble</t>
   </si>
   <si>
-    <t>#vzbp-placeholder &gt; div &gt; div.vzb-tool-stage &gt; div.vzb-tool-viz &gt; div &gt; svg &gt; g &gt; svg.vzb-bc-labels-crop &gt; g.vzb-bc-labels &gt; g &gt; rect</t>
-  </si>
-  <si>
     <t>I can select and deselect countries using the button "Find" to the right.</t>
   </si>
   <si>
@@ -214,6 +211,9 @@
   </si>
   <si>
     <t>Search bar of Find</t>
+  </si>
+  <si>
+    <t>#vzbp-placeholder &gt; div &gt; div.vzb-tool-stage &gt; div.vzb-tool-viz &gt; div &gt; svg &gt; g &gt; svg.vzb-bc-labels-crop &gt; g &gt; g &gt; rect.vzb-label-fill.vzb-tooltip-border</t>
   </si>
 </sst>
 </file>
@@ -336,42 +336,42 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -656,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AA987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34:M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -689,12 +689,12 @@
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -713,16 +713,16 @@
         <v>10</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -739,12 +739,12 @@
       <c r="A9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -762,7 +762,7 @@
       <c r="B11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="12" t="s">
         <v>20</v>
       </c>
     </row>
@@ -770,10 +770,10 @@
       <c r="A12" s="2">
         <v>3</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="12" t="s">
         <v>24</v>
       </c>
     </row>
@@ -781,10 +781,10 @@
       <c r="A13" s="2">
         <v>4</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="12" t="s">
         <v>25</v>
       </c>
     </row>
@@ -792,10 +792,10 @@
       <c r="A14" s="2">
         <v>5</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="12" t="s">
         <v>26</v>
       </c>
     </row>
@@ -803,18 +803,18 @@
       <c r="A16" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>1</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="6"/>
@@ -827,7 +827,7 @@
         <v>10</v>
       </c>
       <c r="C18" s="2"/>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -835,18 +835,18 @@
       <c r="A19" s="10">
         <v>3</v>
       </c>
-      <c r="B19" s="21" t="s">
-        <v>36</v>
+      <c r="B19" s="15" t="s">
+        <v>35</v>
       </c>
       <c r="C19" s="2"/>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
@@ -858,18 +858,18 @@
       <c r="A21" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>1</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="6"/>
@@ -882,7 +882,7 @@
         <v>11</v>
       </c>
       <c r="C23" s="2"/>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -894,17 +894,17 @@
         <v>12</v>
       </c>
       <c r="C24" s="2"/>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
@@ -916,18 +916,18 @@
       <c r="A26" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>1</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="6"/>
@@ -936,39 +936,39 @@
       <c r="A28" s="2">
         <v>2</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="13" t="s">
         <v>28</v>
       </c>
       <c r="C28" s="2"/>
-      <c r="D28" s="16" t="s">
+      <c r="D28" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="16"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
     </row>
     <row r="29" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>3</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="13" t="s">
         <v>30</v>
       </c>
       <c r="C29" s="2"/>
-      <c r="D29" s="15" t="s">
+      <c r="D29" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
@@ -980,18 +980,18 @@
       <c r="A31" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>1</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="6"/>
@@ -1004,7 +1004,7 @@
         <v>11</v>
       </c>
       <c r="C33" s="2"/>
-      <c r="D33" s="19" t="s">
+      <c r="D33" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1012,22 +1012,22 @@
       <c r="A34" s="2">
         <v>3</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C34" s="2"/>
-      <c r="D34" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
-      <c r="M34" s="15"/>
+      <c r="D34" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="21"/>
+      <c r="M34" s="21"/>
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
@@ -1039,18 +1039,18 @@
       <c r="A36" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
+      <c r="B36" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>1</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D37" s="6"/>
@@ -1059,134 +1059,134 @@
       <c r="A38" s="2">
         <v>2</v>
       </c>
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="2"/>
+      <c r="D38" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="15"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="21"/>
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>3</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="2"/>
+      <c r="D39" s="13" t="s">
         <v>39</v>
-      </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="17" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:27" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>4</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="D40" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="22"/>
-      <c r="I40" s="22"/>
-      <c r="J40" s="22"/>
-      <c r="K40" s="22"/>
-      <c r="L40" s="22"/>
-      <c r="M40" s="22"/>
-      <c r="N40" s="22"/>
-      <c r="O40" s="22"/>
-      <c r="P40" s="22"/>
-      <c r="Q40" s="22"/>
-      <c r="R40" s="22"/>
-      <c r="S40" s="22"/>
-      <c r="T40" s="22"/>
-      <c r="U40" s="22"/>
-      <c r="V40" s="22"/>
-      <c r="W40" s="22"/>
-      <c r="X40" s="22"/>
-      <c r="Y40" s="22"/>
-      <c r="Z40" s="22"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
+      <c r="L40" s="19"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="19"/>
+      <c r="O40" s="19"/>
+      <c r="P40" s="19"/>
+      <c r="Q40" s="19"/>
+      <c r="R40" s="19"/>
+      <c r="S40" s="19"/>
+      <c r="T40" s="19"/>
+      <c r="U40" s="19"/>
+      <c r="V40" s="19"/>
+      <c r="W40" s="19"/>
+      <c r="X40" s="19"/>
+      <c r="Y40" s="19"/>
+      <c r="Z40" s="19"/>
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>5</v>
       </c>
-      <c r="B41" s="17" t="s">
-        <v>44</v>
+      <c r="B41" s="13" t="s">
+        <v>43</v>
       </c>
       <c r="C41" s="2"/>
-      <c r="D41" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23"/>
-      <c r="G41" s="23"/>
-      <c r="H41" s="23"/>
-      <c r="I41" s="23"/>
-      <c r="J41" s="23"/>
-      <c r="K41" s="23"/>
-      <c r="L41" s="23"/>
-      <c r="M41" s="23"/>
-      <c r="N41" s="23"/>
-      <c r="O41" s="23"/>
-      <c r="P41" s="23"/>
-      <c r="Q41" s="23"/>
-      <c r="R41" s="23"/>
-      <c r="S41" s="23"/>
-      <c r="T41" s="23"/>
-      <c r="U41" s="23"/>
-      <c r="V41" s="23"/>
-      <c r="W41" s="23"/>
-      <c r="X41" s="23"/>
-      <c r="Y41" s="23"/>
-      <c r="Z41" s="23"/>
-      <c r="AA41" s="23"/>
+      <c r="D41" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="17"/>
+      <c r="J41" s="17"/>
+      <c r="K41" s="17"/>
+      <c r="L41" s="17"/>
+      <c r="M41" s="17"/>
+      <c r="N41" s="17"/>
+      <c r="O41" s="17"/>
+      <c r="P41" s="17"/>
+      <c r="Q41" s="17"/>
+      <c r="R41" s="17"/>
+      <c r="S41" s="17"/>
+      <c r="T41" s="17"/>
+      <c r="U41" s="17"/>
+      <c r="V41" s="17"/>
+      <c r="W41" s="17"/>
+      <c r="X41" s="17"/>
+      <c r="Y41" s="17"/>
+      <c r="Z41" s="17"/>
+      <c r="AA41" s="17"/>
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>6</v>
       </c>
-      <c r="B42" s="17" t="s">
+      <c r="B42" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="E42" s="23"/>
-      <c r="F42" s="23"/>
-      <c r="G42" s="23"/>
-      <c r="H42" s="23"/>
-      <c r="I42" s="23"/>
-      <c r="J42" s="23"/>
-      <c r="K42" s="23"/>
-      <c r="L42" s="23"/>
-      <c r="M42" s="23"/>
-      <c r="N42" s="23"/>
-      <c r="O42" s="23"/>
-      <c r="P42" s="23"/>
-      <c r="Q42" s="23"/>
-      <c r="R42" s="23"/>
-      <c r="S42" s="23"/>
-      <c r="T42" s="23"/>
-      <c r="U42" s="23"/>
-      <c r="V42" s="23"/>
-      <c r="W42" s="23"/>
-      <c r="X42" s="23"/>
-      <c r="Y42" s="23"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="17"/>
+      <c r="K42" s="17"/>
+      <c r="L42" s="17"/>
+      <c r="M42" s="17"/>
+      <c r="N42" s="17"/>
+      <c r="O42" s="17"/>
+      <c r="P42" s="17"/>
+      <c r="Q42" s="17"/>
+      <c r="R42" s="17"/>
+      <c r="S42" s="17"/>
+      <c r="T42" s="17"/>
+      <c r="U42" s="17"/>
+      <c r="V42" s="17"/>
+      <c r="W42" s="17"/>
+      <c r="X42" s="17"/>
+      <c r="Y42" s="17"/>
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" s="10">
@@ -1196,7 +1196,7 @@
         <v>11</v>
       </c>
       <c r="C43" s="2"/>
-      <c r="D43" s="19" t="s">
+      <c r="D43" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1204,25 +1204,25 @@
       <c r="A44" s="2">
         <v>8</v>
       </c>
-      <c r="B44" s="21" t="s">
-        <v>48</v>
+      <c r="B44" s="15" t="s">
+        <v>47</v>
       </c>
       <c r="C44" s="2"/>
-      <c r="D44" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="E44" s="23"/>
-      <c r="F44" s="23"/>
-      <c r="G44" s="23"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
-      <c r="K44" s="23"/>
-      <c r="L44" s="23"/>
-      <c r="M44" s="23"/>
-      <c r="N44" s="23"/>
-      <c r="O44" s="23"/>
-      <c r="P44" s="23"/>
+      <c r="D44" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="17"/>
+      <c r="I44" s="17"/>
+      <c r="J44" s="17"/>
+      <c r="K44" s="17"/>
+      <c r="L44" s="17"/>
+      <c r="M44" s="17"/>
+      <c r="N44" s="17"/>
+      <c r="O44" s="17"/>
+      <c r="P44" s="17"/>
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
@@ -1234,18 +1234,18 @@
       <c r="A46" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
+      <c r="B46" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
     </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>1</v>
       </c>
-      <c r="B47" s="17" t="s">
+      <c r="B47" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D47" s="6"/>
@@ -1254,48 +1254,48 @@
       <c r="A48" s="2">
         <v>2</v>
       </c>
-      <c r="B48" s="17" t="s">
-        <v>59</v>
+      <c r="B48" s="13" t="s">
+        <v>58</v>
       </c>
       <c r="C48" s="2"/>
-      <c r="D48" s="24" t="s">
-        <v>50</v>
+      <c r="D48" s="16" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>3</v>
       </c>
-      <c r="B49" s="17" t="s">
-        <v>64</v>
+      <c r="B49" s="13" t="s">
+        <v>63</v>
       </c>
       <c r="C49" s="2"/>
-      <c r="D49" s="24" t="s">
-        <v>51</v>
+      <c r="D49" s="16" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>4</v>
       </c>
-      <c r="B50" s="17" t="s">
-        <v>44</v>
+      <c r="B50" s="13" t="s">
+        <v>43</v>
       </c>
       <c r="C50" s="2"/>
-      <c r="D50" s="24" t="s">
-        <v>52</v>
+      <c r="D50" s="16" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>5</v>
       </c>
-      <c r="B51" s="17" t="s">
-        <v>45</v>
+      <c r="B51" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="C51" s="2"/>
-      <c r="D51" s="24" t="s">
-        <v>53</v>
+      <c r="D51" s="16" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.25">
@@ -1306,7 +1306,7 @@
         <v>11</v>
       </c>
       <c r="C52" s="2"/>
-      <c r="D52" s="19" t="s">
+      <c r="D52" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1314,31 +1314,31 @@
       <c r="A53" s="2">
         <v>7</v>
       </c>
-      <c r="B53" s="17" t="s">
-        <v>55</v>
+      <c r="B53" s="13" t="s">
+        <v>54</v>
       </c>
       <c r="C53" s="2"/>
-      <c r="D53" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="E53" s="23"/>
-      <c r="F53" s="23"/>
-      <c r="G53" s="23"/>
-      <c r="H53" s="23"/>
-      <c r="I53" s="23"/>
-      <c r="J53" s="23"/>
-      <c r="K53" s="23"/>
+      <c r="D53" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E53" s="17"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="17"/>
+      <c r="I53" s="17"/>
+      <c r="J53" s="17"/>
+      <c r="K53" s="17"/>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>8</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.25">
@@ -1351,18 +1351,18 @@
       <c r="A56" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B56" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C56" s="13"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="13"/>
+      <c r="B56" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>1</v>
       </c>
-      <c r="B57" s="17" t="s">
+      <c r="B57" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D57" s="6"/>
@@ -1371,51 +1371,51 @@
       <c r="A58" s="2">
         <v>2</v>
       </c>
-      <c r="B58" s="17" t="s">
+      <c r="B58" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C58" s="2"/>
+      <c r="D58" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C58" s="2"/>
-      <c r="D58" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="E58" s="23"/>
-      <c r="F58" s="23"/>
-      <c r="G58" s="23"/>
-      <c r="H58" s="23"/>
-      <c r="I58" s="23"/>
-      <c r="J58" s="23"/>
-      <c r="K58" s="23"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="17"/>
+      <c r="H58" s="17"/>
+      <c r="I58" s="17"/>
+      <c r="J58" s="17"/>
+      <c r="K58" s="17"/>
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>3</v>
       </c>
-      <c r="B59" s="17" t="s">
+      <c r="B59" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C59" s="2"/>
+      <c r="D59" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="C59" s="2"/>
-      <c r="D59" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="E59" s="23"/>
-      <c r="F59" s="23"/>
-      <c r="G59" s="23"/>
-      <c r="H59" s="23"/>
-      <c r="I59" s="23"/>
-      <c r="J59" s="23"/>
-      <c r="K59" s="23"/>
-      <c r="L59" s="23"/>
-      <c r="M59" s="23"/>
-      <c r="N59" s="23"/>
-      <c r="O59" s="23"/>
-      <c r="P59" s="23"/>
-      <c r="Q59" s="23"/>
-      <c r="R59" s="23"/>
-      <c r="S59" s="23"/>
-      <c r="T59" s="23"/>
-      <c r="U59" s="23"/>
-      <c r="V59" s="23"/>
-      <c r="W59" s="23"/>
+      <c r="E59" s="17"/>
+      <c r="F59" s="17"/>
+      <c r="G59" s="17"/>
+      <c r="H59" s="17"/>
+      <c r="I59" s="17"/>
+      <c r="J59" s="17"/>
+      <c r="K59" s="17"/>
+      <c r="L59" s="17"/>
+      <c r="M59" s="17"/>
+      <c r="N59" s="17"/>
+      <c r="O59" s="17"/>
+      <c r="P59" s="17"/>
+      <c r="Q59" s="17"/>
+      <c r="R59" s="17"/>
+      <c r="S59" s="17"/>
+      <c r="T59" s="17"/>
+      <c r="U59" s="17"/>
+      <c r="V59" s="17"/>
+      <c r="W59" s="17"/>
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
@@ -1425,107 +1425,107 @@
     </row>
     <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
-      <c r="B61" s="17"/>
+      <c r="B61" s="13"/>
       <c r="D61" s="6"/>
     </row>
     <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
       <c r="B62" s="9"/>
       <c r="C62" s="2"/>
-      <c r="D62" s="19"/>
+      <c r="D62" s="14"/>
     </row>
     <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
-      <c r="B63" s="17"/>
+      <c r="B63" s="13"/>
       <c r="C63" s="2"/>
-      <c r="D63" s="23"/>
-      <c r="E63" s="23"/>
-      <c r="F63" s="23"/>
-      <c r="G63" s="23"/>
-      <c r="H63" s="23"/>
-      <c r="I63" s="23"/>
-      <c r="J63" s="23"/>
-      <c r="K63" s="23"/>
-      <c r="L63" s="23"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="17"/>
+      <c r="F63" s="17"/>
+      <c r="G63" s="17"/>
+      <c r="H63" s="17"/>
+      <c r="I63" s="17"/>
+      <c r="J63" s="17"/>
+      <c r="K63" s="17"/>
+      <c r="L63" s="17"/>
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
-      <c r="B64" s="17"/>
+      <c r="B64" s="13"/>
       <c r="C64" s="2"/>
-      <c r="D64" s="23"/>
-      <c r="E64" s="23"/>
-      <c r="F64" s="23"/>
-      <c r="G64" s="23"/>
-      <c r="H64" s="23"/>
-      <c r="I64" s="23"/>
-      <c r="J64" s="23"/>
-      <c r="K64" s="23"/>
-      <c r="L64" s="23"/>
-      <c r="M64" s="23"/>
-      <c r="N64" s="23"/>
-      <c r="O64" s="23"/>
-      <c r="P64" s="23"/>
-      <c r="Q64" s="23"/>
-      <c r="R64" s="23"/>
-      <c r="S64" s="23"/>
-      <c r="T64" s="23"/>
-      <c r="U64" s="23"/>
-      <c r="V64" s="23"/>
-      <c r="W64" s="23"/>
+      <c r="D64" s="17"/>
+      <c r="E64" s="17"/>
+      <c r="F64" s="17"/>
+      <c r="G64" s="17"/>
+      <c r="H64" s="17"/>
+      <c r="I64" s="17"/>
+      <c r="J64" s="17"/>
+      <c r="K64" s="17"/>
+      <c r="L64" s="17"/>
+      <c r="M64" s="17"/>
+      <c r="N64" s="17"/>
+      <c r="O64" s="17"/>
+      <c r="P64" s="17"/>
+      <c r="Q64" s="17"/>
+      <c r="R64" s="17"/>
+      <c r="S64" s="17"/>
+      <c r="T64" s="17"/>
+      <c r="U64" s="17"/>
+      <c r="V64" s="17"/>
+      <c r="W64" s="17"/>
     </row>
     <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
-      <c r="B65" s="17"/>
+      <c r="B65" s="13"/>
       <c r="C65" s="2"/>
       <c r="D65" s="4"/>
     </row>
     <row r="66" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
-      <c r="B66" s="17"/>
+      <c r="B66" s="13"/>
       <c r="C66" s="2"/>
-      <c r="D66" s="23"/>
-      <c r="E66" s="23"/>
-      <c r="F66" s="23"/>
-      <c r="G66" s="23"/>
-      <c r="H66" s="23"/>
-      <c r="I66" s="23"/>
-      <c r="J66" s="23"/>
-      <c r="K66" s="23"/>
-      <c r="L66" s="23"/>
-      <c r="M66" s="23"/>
-      <c r="N66" s="23"/>
-      <c r="O66" s="23"/>
-      <c r="P66" s="23"/>
-      <c r="Q66" s="23"/>
-      <c r="R66" s="23"/>
-      <c r="S66" s="23"/>
-      <c r="T66" s="23"/>
-      <c r="U66" s="23"/>
-      <c r="V66" s="23"/>
-      <c r="W66" s="23"/>
-      <c r="X66" s="23"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="17"/>
+      <c r="F66" s="17"/>
+      <c r="G66" s="17"/>
+      <c r="H66" s="17"/>
+      <c r="I66" s="17"/>
+      <c r="J66" s="17"/>
+      <c r="K66" s="17"/>
+      <c r="L66" s="17"/>
+      <c r="M66" s="17"/>
+      <c r="N66" s="17"/>
+      <c r="O66" s="17"/>
+      <c r="P66" s="17"/>
+      <c r="Q66" s="17"/>
+      <c r="R66" s="17"/>
+      <c r="S66" s="17"/>
+      <c r="T66" s="17"/>
+      <c r="U66" s="17"/>
+      <c r="V66" s="17"/>
+      <c r="W66" s="17"/>
+      <c r="X66" s="17"/>
     </row>
     <row r="67" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
-      <c r="B67" s="17"/>
+      <c r="B67" s="13"/>
       <c r="C67" s="2"/>
-      <c r="D67" s="23"/>
-      <c r="E67" s="23"/>
-      <c r="F67" s="23"/>
-      <c r="G67" s="23"/>
-      <c r="H67" s="23"/>
-      <c r="I67" s="23"/>
-      <c r="J67" s="23"/>
-      <c r="K67" s="23"/>
-      <c r="L67" s="23"/>
-      <c r="M67" s="23"/>
-      <c r="N67" s="23"/>
-      <c r="O67" s="23"/>
-      <c r="P67" s="23"/>
-      <c r="Q67" s="23"/>
-      <c r="R67" s="23"/>
-      <c r="S67" s="23"/>
-      <c r="T67" s="23"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="17"/>
+      <c r="F67" s="17"/>
+      <c r="G67" s="17"/>
+      <c r="H67" s="17"/>
+      <c r="I67" s="17"/>
+      <c r="J67" s="17"/>
+      <c r="K67" s="17"/>
+      <c r="L67" s="17"/>
+      <c r="M67" s="17"/>
+      <c r="N67" s="17"/>
+      <c r="O67" s="17"/>
+      <c r="P67" s="17"/>
+      <c r="Q67" s="17"/>
+      <c r="R67" s="17"/>
+      <c r="S67" s="17"/>
+      <c r="T67" s="17"/>
     </row>
     <row r="68" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
@@ -7049,19 +7049,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="D63:L63"/>
-    <mergeCell ref="D64:W64"/>
-    <mergeCell ref="D66:X66"/>
-    <mergeCell ref="D67:T67"/>
-    <mergeCell ref="D53:K53"/>
-    <mergeCell ref="B56:E56"/>
-    <mergeCell ref="D58:K58"/>
-    <mergeCell ref="D59:W59"/>
-    <mergeCell ref="D41:AA41"/>
-    <mergeCell ref="D42:Y42"/>
-    <mergeCell ref="D44:P44"/>
-    <mergeCell ref="B46:E46"/>
-    <mergeCell ref="D40:Z40"/>
     <mergeCell ref="B31:E31"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D34:M34"/>
@@ -7077,6 +7064,19 @@
     <mergeCell ref="D6:K6"/>
     <mergeCell ref="D19:I19"/>
     <mergeCell ref="B4:E4"/>
+    <mergeCell ref="D41:AA41"/>
+    <mergeCell ref="D42:Y42"/>
+    <mergeCell ref="D44:P44"/>
+    <mergeCell ref="B46:E46"/>
+    <mergeCell ref="D40:Z40"/>
+    <mergeCell ref="D63:L63"/>
+    <mergeCell ref="D64:W64"/>
+    <mergeCell ref="D66:X66"/>
+    <mergeCell ref="D67:T67"/>
+    <mergeCell ref="D53:K53"/>
+    <mergeCell ref="B56:E56"/>
+    <mergeCell ref="D58:K58"/>
+    <mergeCell ref="D59:W59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Specs/updated core interactions (#1806)
* Locator of label is changed.

* updated locators in sample excel file

* Testing on Travis after some changes of axis values and increase in wait for element visibility.

* Again testing on travis after some changes to have same resulte locally and on travis.

* Testing on travis to have same results locally and on travis

* Testing on travis after changing execution line of specs files.

* Just testing travis related issues

* Just testing on travis

* Testing

* Testing

* Test

* Testing

* Testing

* Testing

* Testing

* Testing

* Testing

* Testing

* Test

* Test

* Testing

* Testing

* Testing

* Testing

* Test

* Test

* Test

* Test

* Test

* Test

* Test

* Locators changes for bubble map chart (Testing)

* Test

* Testing

* Test

* Travis related issue is fixed
</commit_message>
<xml_diff>
--- a/CoreInteractions_Specs.xlsx
+++ b/CoreInteractions_Specs.xlsx
@@ -123,9 +123,6 @@
     <t>tooltip of selected bubble</t>
   </si>
   <si>
-    <t>#vzbp-placeholder &gt; div &gt; div.vzb-tool-stage &gt; div.vzb-tool-viz &gt; div &gt; svg &gt; g &gt; svg.vzb-bc-labels-crop &gt; g.vzb-bc-labels &gt; g &gt; rect</t>
-  </si>
-  <si>
     <t>I can select and deselect countries using the button "Find" to the right.</t>
   </si>
   <si>
@@ -214,6 +211,9 @@
   </si>
   <si>
     <t>Search bar of Find</t>
+  </si>
+  <si>
+    <t>#vzbp-placeholder &gt; div &gt; div.vzb-tool-stage &gt; div.vzb-tool-viz &gt; div &gt; svg &gt; g &gt; svg.vzb-bc-labels-crop &gt; g &gt; g &gt; rect.vzb-label-fill.vzb-tooltip-border</t>
   </si>
 </sst>
 </file>
@@ -336,42 +336,42 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -656,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AA987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34:M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -689,12 +689,12 @@
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -713,16 +713,16 @@
         <v>10</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -739,12 +739,12 @@
       <c r="A9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -762,7 +762,7 @@
       <c r="B11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="12" t="s">
         <v>20</v>
       </c>
     </row>
@@ -770,10 +770,10 @@
       <c r="A12" s="2">
         <v>3</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="12" t="s">
         <v>24</v>
       </c>
     </row>
@@ -781,10 +781,10 @@
       <c r="A13" s="2">
         <v>4</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="12" t="s">
         <v>25</v>
       </c>
     </row>
@@ -792,10 +792,10 @@
       <c r="A14" s="2">
         <v>5</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="12" t="s">
         <v>26</v>
       </c>
     </row>
@@ -803,18 +803,18 @@
       <c r="A16" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>1</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="6"/>
@@ -827,7 +827,7 @@
         <v>10</v>
       </c>
       <c r="C18" s="2"/>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -835,18 +835,18 @@
       <c r="A19" s="10">
         <v>3</v>
       </c>
-      <c r="B19" s="21" t="s">
-        <v>36</v>
+      <c r="B19" s="15" t="s">
+        <v>35</v>
       </c>
       <c r="C19" s="2"/>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
@@ -858,18 +858,18 @@
       <c r="A21" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>1</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="6"/>
@@ -882,7 +882,7 @@
         <v>11</v>
       </c>
       <c r="C23" s="2"/>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -894,17 +894,17 @@
         <v>12</v>
       </c>
       <c r="C24" s="2"/>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
@@ -916,18 +916,18 @@
       <c r="A26" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>1</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="6"/>
@@ -936,39 +936,39 @@
       <c r="A28" s="2">
         <v>2</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="13" t="s">
         <v>28</v>
       </c>
       <c r="C28" s="2"/>
-      <c r="D28" s="16" t="s">
+      <c r="D28" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="16"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
     </row>
     <row r="29" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>3</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="13" t="s">
         <v>30</v>
       </c>
       <c r="C29" s="2"/>
-      <c r="D29" s="15" t="s">
+      <c r="D29" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
@@ -980,18 +980,18 @@
       <c r="A31" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>1</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="6"/>
@@ -1004,7 +1004,7 @@
         <v>11</v>
       </c>
       <c r="C33" s="2"/>
-      <c r="D33" s="19" t="s">
+      <c r="D33" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1012,22 +1012,22 @@
       <c r="A34" s="2">
         <v>3</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C34" s="2"/>
-      <c r="D34" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
-      <c r="M34" s="15"/>
+      <c r="D34" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="21"/>
+      <c r="M34" s="21"/>
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
@@ -1039,18 +1039,18 @@
       <c r="A36" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
+      <c r="B36" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>1</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D37" s="6"/>
@@ -1059,134 +1059,134 @@
       <c r="A38" s="2">
         <v>2</v>
       </c>
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="2"/>
+      <c r="D38" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="15"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="21"/>
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>3</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="2"/>
+      <c r="D39" s="13" t="s">
         <v>39</v>
-      </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="17" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:27" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>4</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="D40" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="22"/>
-      <c r="I40" s="22"/>
-      <c r="J40" s="22"/>
-      <c r="K40" s="22"/>
-      <c r="L40" s="22"/>
-      <c r="M40" s="22"/>
-      <c r="N40" s="22"/>
-      <c r="O40" s="22"/>
-      <c r="P40" s="22"/>
-      <c r="Q40" s="22"/>
-      <c r="R40" s="22"/>
-      <c r="S40" s="22"/>
-      <c r="T40" s="22"/>
-      <c r="U40" s="22"/>
-      <c r="V40" s="22"/>
-      <c r="W40" s="22"/>
-      <c r="X40" s="22"/>
-      <c r="Y40" s="22"/>
-      <c r="Z40" s="22"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
+      <c r="L40" s="19"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="19"/>
+      <c r="O40" s="19"/>
+      <c r="P40" s="19"/>
+      <c r="Q40" s="19"/>
+      <c r="R40" s="19"/>
+      <c r="S40" s="19"/>
+      <c r="T40" s="19"/>
+      <c r="U40" s="19"/>
+      <c r="V40" s="19"/>
+      <c r="W40" s="19"/>
+      <c r="X40" s="19"/>
+      <c r="Y40" s="19"/>
+      <c r="Z40" s="19"/>
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>5</v>
       </c>
-      <c r="B41" s="17" t="s">
-        <v>44</v>
+      <c r="B41" s="13" t="s">
+        <v>43</v>
       </c>
       <c r="C41" s="2"/>
-      <c r="D41" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23"/>
-      <c r="G41" s="23"/>
-      <c r="H41" s="23"/>
-      <c r="I41" s="23"/>
-      <c r="J41" s="23"/>
-      <c r="K41" s="23"/>
-      <c r="L41" s="23"/>
-      <c r="M41" s="23"/>
-      <c r="N41" s="23"/>
-      <c r="O41" s="23"/>
-      <c r="P41" s="23"/>
-      <c r="Q41" s="23"/>
-      <c r="R41" s="23"/>
-      <c r="S41" s="23"/>
-      <c r="T41" s="23"/>
-      <c r="U41" s="23"/>
-      <c r="V41" s="23"/>
-      <c r="W41" s="23"/>
-      <c r="X41" s="23"/>
-      <c r="Y41" s="23"/>
-      <c r="Z41" s="23"/>
-      <c r="AA41" s="23"/>
+      <c r="D41" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="17"/>
+      <c r="J41" s="17"/>
+      <c r="K41" s="17"/>
+      <c r="L41" s="17"/>
+      <c r="M41" s="17"/>
+      <c r="N41" s="17"/>
+      <c r="O41" s="17"/>
+      <c r="P41" s="17"/>
+      <c r="Q41" s="17"/>
+      <c r="R41" s="17"/>
+      <c r="S41" s="17"/>
+      <c r="T41" s="17"/>
+      <c r="U41" s="17"/>
+      <c r="V41" s="17"/>
+      <c r="W41" s="17"/>
+      <c r="X41" s="17"/>
+      <c r="Y41" s="17"/>
+      <c r="Z41" s="17"/>
+      <c r="AA41" s="17"/>
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>6</v>
       </c>
-      <c r="B42" s="17" t="s">
+      <c r="B42" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="E42" s="23"/>
-      <c r="F42" s="23"/>
-      <c r="G42" s="23"/>
-      <c r="H42" s="23"/>
-      <c r="I42" s="23"/>
-      <c r="J42" s="23"/>
-      <c r="K42" s="23"/>
-      <c r="L42" s="23"/>
-      <c r="M42" s="23"/>
-      <c r="N42" s="23"/>
-      <c r="O42" s="23"/>
-      <c r="P42" s="23"/>
-      <c r="Q42" s="23"/>
-      <c r="R42" s="23"/>
-      <c r="S42" s="23"/>
-      <c r="T42" s="23"/>
-      <c r="U42" s="23"/>
-      <c r="V42" s="23"/>
-      <c r="W42" s="23"/>
-      <c r="X42" s="23"/>
-      <c r="Y42" s="23"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="17"/>
+      <c r="K42" s="17"/>
+      <c r="L42" s="17"/>
+      <c r="M42" s="17"/>
+      <c r="N42" s="17"/>
+      <c r="O42" s="17"/>
+      <c r="P42" s="17"/>
+      <c r="Q42" s="17"/>
+      <c r="R42" s="17"/>
+      <c r="S42" s="17"/>
+      <c r="T42" s="17"/>
+      <c r="U42" s="17"/>
+      <c r="V42" s="17"/>
+      <c r="W42" s="17"/>
+      <c r="X42" s="17"/>
+      <c r="Y42" s="17"/>
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" s="10">
@@ -1196,7 +1196,7 @@
         <v>11</v>
       </c>
       <c r="C43" s="2"/>
-      <c r="D43" s="19" t="s">
+      <c r="D43" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1204,25 +1204,25 @@
       <c r="A44" s="2">
         <v>8</v>
       </c>
-      <c r="B44" s="21" t="s">
-        <v>48</v>
+      <c r="B44" s="15" t="s">
+        <v>47</v>
       </c>
       <c r="C44" s="2"/>
-      <c r="D44" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="E44" s="23"/>
-      <c r="F44" s="23"/>
-      <c r="G44" s="23"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
-      <c r="K44" s="23"/>
-      <c r="L44" s="23"/>
-      <c r="M44" s="23"/>
-      <c r="N44" s="23"/>
-      <c r="O44" s="23"/>
-      <c r="P44" s="23"/>
+      <c r="D44" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="17"/>
+      <c r="I44" s="17"/>
+      <c r="J44" s="17"/>
+      <c r="K44" s="17"/>
+      <c r="L44" s="17"/>
+      <c r="M44" s="17"/>
+      <c r="N44" s="17"/>
+      <c r="O44" s="17"/>
+      <c r="P44" s="17"/>
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
@@ -1234,18 +1234,18 @@
       <c r="A46" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
+      <c r="B46" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
     </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>1</v>
       </c>
-      <c r="B47" s="17" t="s">
+      <c r="B47" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D47" s="6"/>
@@ -1254,48 +1254,48 @@
       <c r="A48" s="2">
         <v>2</v>
       </c>
-      <c r="B48" s="17" t="s">
-        <v>59</v>
+      <c r="B48" s="13" t="s">
+        <v>58</v>
       </c>
       <c r="C48" s="2"/>
-      <c r="D48" s="24" t="s">
-        <v>50</v>
+      <c r="D48" s="16" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>3</v>
       </c>
-      <c r="B49" s="17" t="s">
-        <v>64</v>
+      <c r="B49" s="13" t="s">
+        <v>63</v>
       </c>
       <c r="C49" s="2"/>
-      <c r="D49" s="24" t="s">
-        <v>51</v>
+      <c r="D49" s="16" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>4</v>
       </c>
-      <c r="B50" s="17" t="s">
-        <v>44</v>
+      <c r="B50" s="13" t="s">
+        <v>43</v>
       </c>
       <c r="C50" s="2"/>
-      <c r="D50" s="24" t="s">
-        <v>52</v>
+      <c r="D50" s="16" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>5</v>
       </c>
-      <c r="B51" s="17" t="s">
-        <v>45</v>
+      <c r="B51" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="C51" s="2"/>
-      <c r="D51" s="24" t="s">
-        <v>53</v>
+      <c r="D51" s="16" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.25">
@@ -1306,7 +1306,7 @@
         <v>11</v>
       </c>
       <c r="C52" s="2"/>
-      <c r="D52" s="19" t="s">
+      <c r="D52" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1314,31 +1314,31 @@
       <c r="A53" s="2">
         <v>7</v>
       </c>
-      <c r="B53" s="17" t="s">
-        <v>55</v>
+      <c r="B53" s="13" t="s">
+        <v>54</v>
       </c>
       <c r="C53" s="2"/>
-      <c r="D53" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="E53" s="23"/>
-      <c r="F53" s="23"/>
-      <c r="G53" s="23"/>
-      <c r="H53" s="23"/>
-      <c r="I53" s="23"/>
-      <c r="J53" s="23"/>
-      <c r="K53" s="23"/>
+      <c r="D53" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E53" s="17"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="17"/>
+      <c r="I53" s="17"/>
+      <c r="J53" s="17"/>
+      <c r="K53" s="17"/>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>8</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.25">
@@ -1351,18 +1351,18 @@
       <c r="A56" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B56" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C56" s="13"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="13"/>
+      <c r="B56" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>1</v>
       </c>
-      <c r="B57" s="17" t="s">
+      <c r="B57" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D57" s="6"/>
@@ -1371,51 +1371,51 @@
       <c r="A58" s="2">
         <v>2</v>
       </c>
-      <c r="B58" s="17" t="s">
+      <c r="B58" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C58" s="2"/>
+      <c r="D58" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C58" s="2"/>
-      <c r="D58" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="E58" s="23"/>
-      <c r="F58" s="23"/>
-      <c r="G58" s="23"/>
-      <c r="H58" s="23"/>
-      <c r="I58" s="23"/>
-      <c r="J58" s="23"/>
-      <c r="K58" s="23"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="17"/>
+      <c r="H58" s="17"/>
+      <c r="I58" s="17"/>
+      <c r="J58" s="17"/>
+      <c r="K58" s="17"/>
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>3</v>
       </c>
-      <c r="B59" s="17" t="s">
+      <c r="B59" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C59" s="2"/>
+      <c r="D59" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="C59" s="2"/>
-      <c r="D59" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="E59" s="23"/>
-      <c r="F59" s="23"/>
-      <c r="G59" s="23"/>
-      <c r="H59" s="23"/>
-      <c r="I59" s="23"/>
-      <c r="J59" s="23"/>
-      <c r="K59" s="23"/>
-      <c r="L59" s="23"/>
-      <c r="M59" s="23"/>
-      <c r="N59" s="23"/>
-      <c r="O59" s="23"/>
-      <c r="P59" s="23"/>
-      <c r="Q59" s="23"/>
-      <c r="R59" s="23"/>
-      <c r="S59" s="23"/>
-      <c r="T59" s="23"/>
-      <c r="U59" s="23"/>
-      <c r="V59" s="23"/>
-      <c r="W59" s="23"/>
+      <c r="E59" s="17"/>
+      <c r="F59" s="17"/>
+      <c r="G59" s="17"/>
+      <c r="H59" s="17"/>
+      <c r="I59" s="17"/>
+      <c r="J59" s="17"/>
+      <c r="K59" s="17"/>
+      <c r="L59" s="17"/>
+      <c r="M59" s="17"/>
+      <c r="N59" s="17"/>
+      <c r="O59" s="17"/>
+      <c r="P59" s="17"/>
+      <c r="Q59" s="17"/>
+      <c r="R59" s="17"/>
+      <c r="S59" s="17"/>
+      <c r="T59" s="17"/>
+      <c r="U59" s="17"/>
+      <c r="V59" s="17"/>
+      <c r="W59" s="17"/>
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
@@ -1425,107 +1425,107 @@
     </row>
     <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
-      <c r="B61" s="17"/>
+      <c r="B61" s="13"/>
       <c r="D61" s="6"/>
     </row>
     <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
       <c r="B62" s="9"/>
       <c r="C62" s="2"/>
-      <c r="D62" s="19"/>
+      <c r="D62" s="14"/>
     </row>
     <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
-      <c r="B63" s="17"/>
+      <c r="B63" s="13"/>
       <c r="C63" s="2"/>
-      <c r="D63" s="23"/>
-      <c r="E63" s="23"/>
-      <c r="F63" s="23"/>
-      <c r="G63" s="23"/>
-      <c r="H63" s="23"/>
-      <c r="I63" s="23"/>
-      <c r="J63" s="23"/>
-      <c r="K63" s="23"/>
-      <c r="L63" s="23"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="17"/>
+      <c r="F63" s="17"/>
+      <c r="G63" s="17"/>
+      <c r="H63" s="17"/>
+      <c r="I63" s="17"/>
+      <c r="J63" s="17"/>
+      <c r="K63" s="17"/>
+      <c r="L63" s="17"/>
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
-      <c r="B64" s="17"/>
+      <c r="B64" s="13"/>
       <c r="C64" s="2"/>
-      <c r="D64" s="23"/>
-      <c r="E64" s="23"/>
-      <c r="F64" s="23"/>
-      <c r="G64" s="23"/>
-      <c r="H64" s="23"/>
-      <c r="I64" s="23"/>
-      <c r="J64" s="23"/>
-      <c r="K64" s="23"/>
-      <c r="L64" s="23"/>
-      <c r="M64" s="23"/>
-      <c r="N64" s="23"/>
-      <c r="O64" s="23"/>
-      <c r="P64" s="23"/>
-      <c r="Q64" s="23"/>
-      <c r="R64" s="23"/>
-      <c r="S64" s="23"/>
-      <c r="T64" s="23"/>
-      <c r="U64" s="23"/>
-      <c r="V64" s="23"/>
-      <c r="W64" s="23"/>
+      <c r="D64" s="17"/>
+      <c r="E64" s="17"/>
+      <c r="F64" s="17"/>
+      <c r="G64" s="17"/>
+      <c r="H64" s="17"/>
+      <c r="I64" s="17"/>
+      <c r="J64" s="17"/>
+      <c r="K64" s="17"/>
+      <c r="L64" s="17"/>
+      <c r="M64" s="17"/>
+      <c r="N64" s="17"/>
+      <c r="O64" s="17"/>
+      <c r="P64" s="17"/>
+      <c r="Q64" s="17"/>
+      <c r="R64" s="17"/>
+      <c r="S64" s="17"/>
+      <c r="T64" s="17"/>
+      <c r="U64" s="17"/>
+      <c r="V64" s="17"/>
+      <c r="W64" s="17"/>
     </row>
     <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
-      <c r="B65" s="17"/>
+      <c r="B65" s="13"/>
       <c r="C65" s="2"/>
       <c r="D65" s="4"/>
     </row>
     <row r="66" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
-      <c r="B66" s="17"/>
+      <c r="B66" s="13"/>
       <c r="C66" s="2"/>
-      <c r="D66" s="23"/>
-      <c r="E66" s="23"/>
-      <c r="F66" s="23"/>
-      <c r="G66" s="23"/>
-      <c r="H66" s="23"/>
-      <c r="I66" s="23"/>
-      <c r="J66" s="23"/>
-      <c r="K66" s="23"/>
-      <c r="L66" s="23"/>
-      <c r="M66" s="23"/>
-      <c r="N66" s="23"/>
-      <c r="O66" s="23"/>
-      <c r="P66" s="23"/>
-      <c r="Q66" s="23"/>
-      <c r="R66" s="23"/>
-      <c r="S66" s="23"/>
-      <c r="T66" s="23"/>
-      <c r="U66" s="23"/>
-      <c r="V66" s="23"/>
-      <c r="W66" s="23"/>
-      <c r="X66" s="23"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="17"/>
+      <c r="F66" s="17"/>
+      <c r="G66" s="17"/>
+      <c r="H66" s="17"/>
+      <c r="I66" s="17"/>
+      <c r="J66" s="17"/>
+      <c r="K66" s="17"/>
+      <c r="L66" s="17"/>
+      <c r="M66" s="17"/>
+      <c r="N66" s="17"/>
+      <c r="O66" s="17"/>
+      <c r="P66" s="17"/>
+      <c r="Q66" s="17"/>
+      <c r="R66" s="17"/>
+      <c r="S66" s="17"/>
+      <c r="T66" s="17"/>
+      <c r="U66" s="17"/>
+      <c r="V66" s="17"/>
+      <c r="W66" s="17"/>
+      <c r="X66" s="17"/>
     </row>
     <row r="67" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
-      <c r="B67" s="17"/>
+      <c r="B67" s="13"/>
       <c r="C67" s="2"/>
-      <c r="D67" s="23"/>
-      <c r="E67" s="23"/>
-      <c r="F67" s="23"/>
-      <c r="G67" s="23"/>
-      <c r="H67" s="23"/>
-      <c r="I67" s="23"/>
-      <c r="J67" s="23"/>
-      <c r="K67" s="23"/>
-      <c r="L67" s="23"/>
-      <c r="M67" s="23"/>
-      <c r="N67" s="23"/>
-      <c r="O67" s="23"/>
-      <c r="P67" s="23"/>
-      <c r="Q67" s="23"/>
-      <c r="R67" s="23"/>
-      <c r="S67" s="23"/>
-      <c r="T67" s="23"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="17"/>
+      <c r="F67" s="17"/>
+      <c r="G67" s="17"/>
+      <c r="H67" s="17"/>
+      <c r="I67" s="17"/>
+      <c r="J67" s="17"/>
+      <c r="K67" s="17"/>
+      <c r="L67" s="17"/>
+      <c r="M67" s="17"/>
+      <c r="N67" s="17"/>
+      <c r="O67" s="17"/>
+      <c r="P67" s="17"/>
+      <c r="Q67" s="17"/>
+      <c r="R67" s="17"/>
+      <c r="S67" s="17"/>
+      <c r="T67" s="17"/>
     </row>
     <row r="68" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
@@ -7049,19 +7049,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="D63:L63"/>
-    <mergeCell ref="D64:W64"/>
-    <mergeCell ref="D66:X66"/>
-    <mergeCell ref="D67:T67"/>
-    <mergeCell ref="D53:K53"/>
-    <mergeCell ref="B56:E56"/>
-    <mergeCell ref="D58:K58"/>
-    <mergeCell ref="D59:W59"/>
-    <mergeCell ref="D41:AA41"/>
-    <mergeCell ref="D42:Y42"/>
-    <mergeCell ref="D44:P44"/>
-    <mergeCell ref="B46:E46"/>
-    <mergeCell ref="D40:Z40"/>
     <mergeCell ref="B31:E31"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D34:M34"/>
@@ -7077,6 +7064,19 @@
     <mergeCell ref="D6:K6"/>
     <mergeCell ref="D19:I19"/>
     <mergeCell ref="B4:E4"/>
+    <mergeCell ref="D41:AA41"/>
+    <mergeCell ref="D42:Y42"/>
+    <mergeCell ref="D44:P44"/>
+    <mergeCell ref="B46:E46"/>
+    <mergeCell ref="D40:Z40"/>
+    <mergeCell ref="D63:L63"/>
+    <mergeCell ref="D64:W64"/>
+    <mergeCell ref="D66:X66"/>
+    <mergeCell ref="D67:T67"/>
+    <mergeCell ref="D53:K53"/>
+    <mergeCell ref="B56:E56"/>
+    <mergeCell ref="D58:K58"/>
+    <mergeCell ref="D59:W59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Specs/updated core interactions (#1806) (#1807)
* Locator of label is changed.

* updated locators in sample excel file

* Testing on Travis after some changes of axis values and increase in wait for element visibility.

* Again testing on travis after some changes to have same resulte locally and on travis.

* Testing on travis to have same results locally and on travis

* Testing on travis after changing execution line of specs files.

* Just testing travis related issues

* Just testing on travis

* Testing

* Testing

* Test

* Testing

* Testing

* Testing

* Testing

* Testing

* Testing

* Testing

* Test

* Test

* Testing

* Testing

* Testing

* Testing

* Test

* Test

* Test

* Test

* Test

* Test

* Test

* Locators changes for bubble map chart (Testing)

* Test

* Testing

* Test

* Travis related issue is fixed
</commit_message>
<xml_diff>
--- a/CoreInteractions_Specs.xlsx
+++ b/CoreInteractions_Specs.xlsx
@@ -123,9 +123,6 @@
     <t>tooltip of selected bubble</t>
   </si>
   <si>
-    <t>#vzbp-placeholder &gt; div &gt; div.vzb-tool-stage &gt; div.vzb-tool-viz &gt; div &gt; svg &gt; g &gt; svg.vzb-bc-labels-crop &gt; g.vzb-bc-labels &gt; g &gt; rect</t>
-  </si>
-  <si>
     <t>I can select and deselect countries using the button "Find" to the right.</t>
   </si>
   <si>
@@ -214,6 +211,9 @@
   </si>
   <si>
     <t>Search bar of Find</t>
+  </si>
+  <si>
+    <t>#vzbp-placeholder &gt; div &gt; div.vzb-tool-stage &gt; div.vzb-tool-viz &gt; div &gt; svg &gt; g &gt; svg.vzb-bc-labels-crop &gt; g &gt; g &gt; rect.vzb-label-fill.vzb-tooltip-border</t>
   </si>
 </sst>
 </file>
@@ -336,42 +336,42 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -656,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AA987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34:M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -689,12 +689,12 @@
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -713,16 +713,16 @@
         <v>10</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -739,12 +739,12 @@
       <c r="A9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -762,7 +762,7 @@
       <c r="B11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="12" t="s">
         <v>20</v>
       </c>
     </row>
@@ -770,10 +770,10 @@
       <c r="A12" s="2">
         <v>3</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="12" t="s">
         <v>24</v>
       </c>
     </row>
@@ -781,10 +781,10 @@
       <c r="A13" s="2">
         <v>4</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="12" t="s">
         <v>25</v>
       </c>
     </row>
@@ -792,10 +792,10 @@
       <c r="A14" s="2">
         <v>5</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="12" t="s">
         <v>26</v>
       </c>
     </row>
@@ -803,18 +803,18 @@
       <c r="A16" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>1</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="6"/>
@@ -827,7 +827,7 @@
         <v>10</v>
       </c>
       <c r="C18" s="2"/>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -835,18 +835,18 @@
       <c r="A19" s="10">
         <v>3</v>
       </c>
-      <c r="B19" s="21" t="s">
-        <v>36</v>
+      <c r="B19" s="15" t="s">
+        <v>35</v>
       </c>
       <c r="C19" s="2"/>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
@@ -858,18 +858,18 @@
       <c r="A21" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>1</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="6"/>
@@ -882,7 +882,7 @@
         <v>11</v>
       </c>
       <c r="C23" s="2"/>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -894,17 +894,17 @@
         <v>12</v>
       </c>
       <c r="C24" s="2"/>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
@@ -916,18 +916,18 @@
       <c r="A26" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>1</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="6"/>
@@ -936,39 +936,39 @@
       <c r="A28" s="2">
         <v>2</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="13" t="s">
         <v>28</v>
       </c>
       <c r="C28" s="2"/>
-      <c r="D28" s="16" t="s">
+      <c r="D28" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="16"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
     </row>
     <row r="29" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>3</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="13" t="s">
         <v>30</v>
       </c>
       <c r="C29" s="2"/>
-      <c r="D29" s="15" t="s">
+      <c r="D29" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
@@ -980,18 +980,18 @@
       <c r="A31" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>1</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="6"/>
@@ -1004,7 +1004,7 @@
         <v>11</v>
       </c>
       <c r="C33" s="2"/>
-      <c r="D33" s="19" t="s">
+      <c r="D33" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1012,22 +1012,22 @@
       <c r="A34" s="2">
         <v>3</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C34" s="2"/>
-      <c r="D34" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
-      <c r="M34" s="15"/>
+      <c r="D34" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="21"/>
+      <c r="M34" s="21"/>
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
@@ -1039,18 +1039,18 @@
       <c r="A36" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
+      <c r="B36" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>1</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D37" s="6"/>
@@ -1059,134 +1059,134 @@
       <c r="A38" s="2">
         <v>2</v>
       </c>
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="2"/>
+      <c r="D38" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="15"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="21"/>
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>3</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="2"/>
+      <c r="D39" s="13" t="s">
         <v>39</v>
-      </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="17" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:27" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>4</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="D40" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="22"/>
-      <c r="I40" s="22"/>
-      <c r="J40" s="22"/>
-      <c r="K40" s="22"/>
-      <c r="L40" s="22"/>
-      <c r="M40" s="22"/>
-      <c r="N40" s="22"/>
-      <c r="O40" s="22"/>
-      <c r="P40" s="22"/>
-      <c r="Q40" s="22"/>
-      <c r="R40" s="22"/>
-      <c r="S40" s="22"/>
-      <c r="T40" s="22"/>
-      <c r="U40" s="22"/>
-      <c r="V40" s="22"/>
-      <c r="W40" s="22"/>
-      <c r="X40" s="22"/>
-      <c r="Y40" s="22"/>
-      <c r="Z40" s="22"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
+      <c r="L40" s="19"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="19"/>
+      <c r="O40" s="19"/>
+      <c r="P40" s="19"/>
+      <c r="Q40" s="19"/>
+      <c r="R40" s="19"/>
+      <c r="S40" s="19"/>
+      <c r="T40" s="19"/>
+      <c r="U40" s="19"/>
+      <c r="V40" s="19"/>
+      <c r="W40" s="19"/>
+      <c r="X40" s="19"/>
+      <c r="Y40" s="19"/>
+      <c r="Z40" s="19"/>
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>5</v>
       </c>
-      <c r="B41" s="17" t="s">
-        <v>44</v>
+      <c r="B41" s="13" t="s">
+        <v>43</v>
       </c>
       <c r="C41" s="2"/>
-      <c r="D41" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23"/>
-      <c r="G41" s="23"/>
-      <c r="H41" s="23"/>
-      <c r="I41" s="23"/>
-      <c r="J41" s="23"/>
-      <c r="K41" s="23"/>
-      <c r="L41" s="23"/>
-      <c r="M41" s="23"/>
-      <c r="N41" s="23"/>
-      <c r="O41" s="23"/>
-      <c r="P41" s="23"/>
-      <c r="Q41" s="23"/>
-      <c r="R41" s="23"/>
-      <c r="S41" s="23"/>
-      <c r="T41" s="23"/>
-      <c r="U41" s="23"/>
-      <c r="V41" s="23"/>
-      <c r="W41" s="23"/>
-      <c r="X41" s="23"/>
-      <c r="Y41" s="23"/>
-      <c r="Z41" s="23"/>
-      <c r="AA41" s="23"/>
+      <c r="D41" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="17"/>
+      <c r="J41" s="17"/>
+      <c r="K41" s="17"/>
+      <c r="L41" s="17"/>
+      <c r="M41" s="17"/>
+      <c r="N41" s="17"/>
+      <c r="O41" s="17"/>
+      <c r="P41" s="17"/>
+      <c r="Q41" s="17"/>
+      <c r="R41" s="17"/>
+      <c r="S41" s="17"/>
+      <c r="T41" s="17"/>
+      <c r="U41" s="17"/>
+      <c r="V41" s="17"/>
+      <c r="W41" s="17"/>
+      <c r="X41" s="17"/>
+      <c r="Y41" s="17"/>
+      <c r="Z41" s="17"/>
+      <c r="AA41" s="17"/>
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>6</v>
       </c>
-      <c r="B42" s="17" t="s">
+      <c r="B42" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="E42" s="23"/>
-      <c r="F42" s="23"/>
-      <c r="G42" s="23"/>
-      <c r="H42" s="23"/>
-      <c r="I42" s="23"/>
-      <c r="J42" s="23"/>
-      <c r="K42" s="23"/>
-      <c r="L42" s="23"/>
-      <c r="M42" s="23"/>
-      <c r="N42" s="23"/>
-      <c r="O42" s="23"/>
-      <c r="P42" s="23"/>
-      <c r="Q42" s="23"/>
-      <c r="R42" s="23"/>
-      <c r="S42" s="23"/>
-      <c r="T42" s="23"/>
-      <c r="U42" s="23"/>
-      <c r="V42" s="23"/>
-      <c r="W42" s="23"/>
-      <c r="X42" s="23"/>
-      <c r="Y42" s="23"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="17"/>
+      <c r="K42" s="17"/>
+      <c r="L42" s="17"/>
+      <c r="M42" s="17"/>
+      <c r="N42" s="17"/>
+      <c r="O42" s="17"/>
+      <c r="P42" s="17"/>
+      <c r="Q42" s="17"/>
+      <c r="R42" s="17"/>
+      <c r="S42" s="17"/>
+      <c r="T42" s="17"/>
+      <c r="U42" s="17"/>
+      <c r="V42" s="17"/>
+      <c r="W42" s="17"/>
+      <c r="X42" s="17"/>
+      <c r="Y42" s="17"/>
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" s="10">
@@ -1196,7 +1196,7 @@
         <v>11</v>
       </c>
       <c r="C43" s="2"/>
-      <c r="D43" s="19" t="s">
+      <c r="D43" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1204,25 +1204,25 @@
       <c r="A44" s="2">
         <v>8</v>
       </c>
-      <c r="B44" s="21" t="s">
-        <v>48</v>
+      <c r="B44" s="15" t="s">
+        <v>47</v>
       </c>
       <c r="C44" s="2"/>
-      <c r="D44" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="E44" s="23"/>
-      <c r="F44" s="23"/>
-      <c r="G44" s="23"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
-      <c r="K44" s="23"/>
-      <c r="L44" s="23"/>
-      <c r="M44" s="23"/>
-      <c r="N44" s="23"/>
-      <c r="O44" s="23"/>
-      <c r="P44" s="23"/>
+      <c r="D44" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="17"/>
+      <c r="I44" s="17"/>
+      <c r="J44" s="17"/>
+      <c r="K44" s="17"/>
+      <c r="L44" s="17"/>
+      <c r="M44" s="17"/>
+      <c r="N44" s="17"/>
+      <c r="O44" s="17"/>
+      <c r="P44" s="17"/>
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
@@ -1234,18 +1234,18 @@
       <c r="A46" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
+      <c r="B46" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
     </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>1</v>
       </c>
-      <c r="B47" s="17" t="s">
+      <c r="B47" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D47" s="6"/>
@@ -1254,48 +1254,48 @@
       <c r="A48" s="2">
         <v>2</v>
       </c>
-      <c r="B48" s="17" t="s">
-        <v>59</v>
+      <c r="B48" s="13" t="s">
+        <v>58</v>
       </c>
       <c r="C48" s="2"/>
-      <c r="D48" s="24" t="s">
-        <v>50</v>
+      <c r="D48" s="16" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>3</v>
       </c>
-      <c r="B49" s="17" t="s">
-        <v>64</v>
+      <c r="B49" s="13" t="s">
+        <v>63</v>
       </c>
       <c r="C49" s="2"/>
-      <c r="D49" s="24" t="s">
-        <v>51</v>
+      <c r="D49" s="16" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>4</v>
       </c>
-      <c r="B50" s="17" t="s">
-        <v>44</v>
+      <c r="B50" s="13" t="s">
+        <v>43</v>
       </c>
       <c r="C50" s="2"/>
-      <c r="D50" s="24" t="s">
-        <v>52</v>
+      <c r="D50" s="16" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>5</v>
       </c>
-      <c r="B51" s="17" t="s">
-        <v>45</v>
+      <c r="B51" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="C51" s="2"/>
-      <c r="D51" s="24" t="s">
-        <v>53</v>
+      <c r="D51" s="16" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.25">
@@ -1306,7 +1306,7 @@
         <v>11</v>
       </c>
       <c r="C52" s="2"/>
-      <c r="D52" s="19" t="s">
+      <c r="D52" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1314,31 +1314,31 @@
       <c r="A53" s="2">
         <v>7</v>
       </c>
-      <c r="B53" s="17" t="s">
-        <v>55</v>
+      <c r="B53" s="13" t="s">
+        <v>54</v>
       </c>
       <c r="C53" s="2"/>
-      <c r="D53" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="E53" s="23"/>
-      <c r="F53" s="23"/>
-      <c r="G53" s="23"/>
-      <c r="H53" s="23"/>
-      <c r="I53" s="23"/>
-      <c r="J53" s="23"/>
-      <c r="K53" s="23"/>
+      <c r="D53" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E53" s="17"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="17"/>
+      <c r="I53" s="17"/>
+      <c r="J53" s="17"/>
+      <c r="K53" s="17"/>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>8</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.25">
@@ -1351,18 +1351,18 @@
       <c r="A56" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B56" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C56" s="13"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="13"/>
+      <c r="B56" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>1</v>
       </c>
-      <c r="B57" s="17" t="s">
+      <c r="B57" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D57" s="6"/>
@@ -1371,51 +1371,51 @@
       <c r="A58" s="2">
         <v>2</v>
       </c>
-      <c r="B58" s="17" t="s">
+      <c r="B58" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C58" s="2"/>
+      <c r="D58" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C58" s="2"/>
-      <c r="D58" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="E58" s="23"/>
-      <c r="F58" s="23"/>
-      <c r="G58" s="23"/>
-      <c r="H58" s="23"/>
-      <c r="I58" s="23"/>
-      <c r="J58" s="23"/>
-      <c r="K58" s="23"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="17"/>
+      <c r="H58" s="17"/>
+      <c r="I58" s="17"/>
+      <c r="J58" s="17"/>
+      <c r="K58" s="17"/>
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>3</v>
       </c>
-      <c r="B59" s="17" t="s">
+      <c r="B59" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C59" s="2"/>
+      <c r="D59" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="C59" s="2"/>
-      <c r="D59" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="E59" s="23"/>
-      <c r="F59" s="23"/>
-      <c r="G59" s="23"/>
-      <c r="H59" s="23"/>
-      <c r="I59" s="23"/>
-      <c r="J59" s="23"/>
-      <c r="K59" s="23"/>
-      <c r="L59" s="23"/>
-      <c r="M59" s="23"/>
-      <c r="N59" s="23"/>
-      <c r="O59" s="23"/>
-      <c r="P59" s="23"/>
-      <c r="Q59" s="23"/>
-      <c r="R59" s="23"/>
-      <c r="S59" s="23"/>
-      <c r="T59" s="23"/>
-      <c r="U59" s="23"/>
-      <c r="V59" s="23"/>
-      <c r="W59" s="23"/>
+      <c r="E59" s="17"/>
+      <c r="F59" s="17"/>
+      <c r="G59" s="17"/>
+      <c r="H59" s="17"/>
+      <c r="I59" s="17"/>
+      <c r="J59" s="17"/>
+      <c r="K59" s="17"/>
+      <c r="L59" s="17"/>
+      <c r="M59" s="17"/>
+      <c r="N59" s="17"/>
+      <c r="O59" s="17"/>
+      <c r="P59" s="17"/>
+      <c r="Q59" s="17"/>
+      <c r="R59" s="17"/>
+      <c r="S59" s="17"/>
+      <c r="T59" s="17"/>
+      <c r="U59" s="17"/>
+      <c r="V59" s="17"/>
+      <c r="W59" s="17"/>
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
@@ -1425,107 +1425,107 @@
     </row>
     <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
-      <c r="B61" s="17"/>
+      <c r="B61" s="13"/>
       <c r="D61" s="6"/>
     </row>
     <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
       <c r="B62" s="9"/>
       <c r="C62" s="2"/>
-      <c r="D62" s="19"/>
+      <c r="D62" s="14"/>
     </row>
     <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
-      <c r="B63" s="17"/>
+      <c r="B63" s="13"/>
       <c r="C63" s="2"/>
-      <c r="D63" s="23"/>
-      <c r="E63" s="23"/>
-      <c r="F63" s="23"/>
-      <c r="G63" s="23"/>
-      <c r="H63" s="23"/>
-      <c r="I63" s="23"/>
-      <c r="J63" s="23"/>
-      <c r="K63" s="23"/>
-      <c r="L63" s="23"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="17"/>
+      <c r="F63" s="17"/>
+      <c r="G63" s="17"/>
+      <c r="H63" s="17"/>
+      <c r="I63" s="17"/>
+      <c r="J63" s="17"/>
+      <c r="K63" s="17"/>
+      <c r="L63" s="17"/>
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
-      <c r="B64" s="17"/>
+      <c r="B64" s="13"/>
       <c r="C64" s="2"/>
-      <c r="D64" s="23"/>
-      <c r="E64" s="23"/>
-      <c r="F64" s="23"/>
-      <c r="G64" s="23"/>
-      <c r="H64" s="23"/>
-      <c r="I64" s="23"/>
-      <c r="J64" s="23"/>
-      <c r="K64" s="23"/>
-      <c r="L64" s="23"/>
-      <c r="M64" s="23"/>
-      <c r="N64" s="23"/>
-      <c r="O64" s="23"/>
-      <c r="P64" s="23"/>
-      <c r="Q64" s="23"/>
-      <c r="R64" s="23"/>
-      <c r="S64" s="23"/>
-      <c r="T64" s="23"/>
-      <c r="U64" s="23"/>
-      <c r="V64" s="23"/>
-      <c r="W64" s="23"/>
+      <c r="D64" s="17"/>
+      <c r="E64" s="17"/>
+      <c r="F64" s="17"/>
+      <c r="G64" s="17"/>
+      <c r="H64" s="17"/>
+      <c r="I64" s="17"/>
+      <c r="J64" s="17"/>
+      <c r="K64" s="17"/>
+      <c r="L64" s="17"/>
+      <c r="M64" s="17"/>
+      <c r="N64" s="17"/>
+      <c r="O64" s="17"/>
+      <c r="P64" s="17"/>
+      <c r="Q64" s="17"/>
+      <c r="R64" s="17"/>
+      <c r="S64" s="17"/>
+      <c r="T64" s="17"/>
+      <c r="U64" s="17"/>
+      <c r="V64" s="17"/>
+      <c r="W64" s="17"/>
     </row>
     <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
-      <c r="B65" s="17"/>
+      <c r="B65" s="13"/>
       <c r="C65" s="2"/>
       <c r="D65" s="4"/>
     </row>
     <row r="66" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
-      <c r="B66" s="17"/>
+      <c r="B66" s="13"/>
       <c r="C66" s="2"/>
-      <c r="D66" s="23"/>
-      <c r="E66" s="23"/>
-      <c r="F66" s="23"/>
-      <c r="G66" s="23"/>
-      <c r="H66" s="23"/>
-      <c r="I66" s="23"/>
-      <c r="J66" s="23"/>
-      <c r="K66" s="23"/>
-      <c r="L66" s="23"/>
-      <c r="M66" s="23"/>
-      <c r="N66" s="23"/>
-      <c r="O66" s="23"/>
-      <c r="P66" s="23"/>
-      <c r="Q66" s="23"/>
-      <c r="R66" s="23"/>
-      <c r="S66" s="23"/>
-      <c r="T66" s="23"/>
-      <c r="U66" s="23"/>
-      <c r="V66" s="23"/>
-      <c r="W66" s="23"/>
-      <c r="X66" s="23"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="17"/>
+      <c r="F66" s="17"/>
+      <c r="G66" s="17"/>
+      <c r="H66" s="17"/>
+      <c r="I66" s="17"/>
+      <c r="J66" s="17"/>
+      <c r="K66" s="17"/>
+      <c r="L66" s="17"/>
+      <c r="M66" s="17"/>
+      <c r="N66" s="17"/>
+      <c r="O66" s="17"/>
+      <c r="P66" s="17"/>
+      <c r="Q66" s="17"/>
+      <c r="R66" s="17"/>
+      <c r="S66" s="17"/>
+      <c r="T66" s="17"/>
+      <c r="U66" s="17"/>
+      <c r="V66" s="17"/>
+      <c r="W66" s="17"/>
+      <c r="X66" s="17"/>
     </row>
     <row r="67" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
-      <c r="B67" s="17"/>
+      <c r="B67" s="13"/>
       <c r="C67" s="2"/>
-      <c r="D67" s="23"/>
-      <c r="E67" s="23"/>
-      <c r="F67" s="23"/>
-      <c r="G67" s="23"/>
-      <c r="H67" s="23"/>
-      <c r="I67" s="23"/>
-      <c r="J67" s="23"/>
-      <c r="K67" s="23"/>
-      <c r="L67" s="23"/>
-      <c r="M67" s="23"/>
-      <c r="N67" s="23"/>
-      <c r="O67" s="23"/>
-      <c r="P67" s="23"/>
-      <c r="Q67" s="23"/>
-      <c r="R67" s="23"/>
-      <c r="S67" s="23"/>
-      <c r="T67" s="23"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="17"/>
+      <c r="F67" s="17"/>
+      <c r="G67" s="17"/>
+      <c r="H67" s="17"/>
+      <c r="I67" s="17"/>
+      <c r="J67" s="17"/>
+      <c r="K67" s="17"/>
+      <c r="L67" s="17"/>
+      <c r="M67" s="17"/>
+      <c r="N67" s="17"/>
+      <c r="O67" s="17"/>
+      <c r="P67" s="17"/>
+      <c r="Q67" s="17"/>
+      <c r="R67" s="17"/>
+      <c r="S67" s="17"/>
+      <c r="T67" s="17"/>
     </row>
     <row r="68" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
@@ -7049,19 +7049,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="D63:L63"/>
-    <mergeCell ref="D64:W64"/>
-    <mergeCell ref="D66:X66"/>
-    <mergeCell ref="D67:T67"/>
-    <mergeCell ref="D53:K53"/>
-    <mergeCell ref="B56:E56"/>
-    <mergeCell ref="D58:K58"/>
-    <mergeCell ref="D59:W59"/>
-    <mergeCell ref="D41:AA41"/>
-    <mergeCell ref="D42:Y42"/>
-    <mergeCell ref="D44:P44"/>
-    <mergeCell ref="B46:E46"/>
-    <mergeCell ref="D40:Z40"/>
     <mergeCell ref="B31:E31"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D34:M34"/>
@@ -7077,6 +7064,19 @@
     <mergeCell ref="D6:K6"/>
     <mergeCell ref="D19:I19"/>
     <mergeCell ref="B4:E4"/>
+    <mergeCell ref="D41:AA41"/>
+    <mergeCell ref="D42:Y42"/>
+    <mergeCell ref="D44:P44"/>
+    <mergeCell ref="B46:E46"/>
+    <mergeCell ref="D40:Z40"/>
+    <mergeCell ref="D63:L63"/>
+    <mergeCell ref="D64:W64"/>
+    <mergeCell ref="D66:X66"/>
+    <mergeCell ref="D67:T67"/>
+    <mergeCell ref="D53:K53"/>
+    <mergeCell ref="B56:E56"/>
+    <mergeCell ref="D58:K58"/>
+    <mergeCell ref="D59:W59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>